<commit_message>
Refine the data assembling code, generate dataset ready for modelling in NONMEM
</commit_message>
<xml_diff>
--- a/Datasets/MTT_Erlotinib bio rep 2.xlsx
+++ b/Datasets/MTT_Erlotinib bio rep 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0117675\Documents\DOCTORAAT\Resultaten\WP1 - Aa mutants\Stable ARK1 expressing mutants\Compound treatment\Sophie\Combinaties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/myluong_vuong_kuleuven_be/Documents/PhD in KU Leuven/Projects/Side projects/Cancer Invitro/Report_Oncology_MLV/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D86D0C0-A497-4067-ACCC-3D0C5A8A67AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7D86D0C0-A497-4067-ACCC-3D0C5A8A67AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BC0B71C-8105-493F-996D-6BB18813430A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D45A96DF-C14E-40DC-AD40-F0677B538E27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D45A96DF-C14E-40DC-AD40-F0677B538E27}"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78E36A8-C0A6-4015-81A7-B4FAEE69D0D7}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:J21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,280 +713,280 @@
         <v>97.188628158844764</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <f>175/3</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="C13" s="2">
-        <f>B13/3</f>
+      <c r="C14" s="2">
+        <f>B14/3</f>
         <v>19.444444444444446</v>
       </c>
-      <c r="D13" s="2">
-        <f t="shared" ref="D13:G13" si="2">C13/3</f>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:G14" si="2">C14/3</f>
         <v>6.4814814814814818</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
         <v>2.1604938271604941</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <f t="shared" si="2"/>
         <v>0.72016460905349799</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>0.24005486968449932</v>
       </c>
-      <c r="H13" s="2">
-        <f>G13/3</f>
+      <c r="H14" s="2">
+        <f>G14/3</f>
         <v>8.0018289894833103E-2</v>
       </c>
-      <c r="I13" s="2">
-        <f>H13/3</f>
+      <c r="I14" s="2">
+        <f>H14/3</f>
         <v>2.66727632982777E-2</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>23.55197690759239</v>
-      </c>
-      <c r="C14">
-        <v>31.505184397432494</v>
-      </c>
-      <c r="D14">
-        <v>47.206502335827416</v>
-      </c>
-      <c r="E14">
-        <v>84.24930684796233</v>
-      </c>
-      <c r="F14">
-        <v>101.10144707356908</v>
-      </c>
-      <c r="G14">
-        <v>102.58270348285161</v>
-      </c>
-      <c r="H14">
-        <v>117.65733601731931</v>
-      </c>
-      <c r="I14">
-        <v>102.48015496220897</v>
-      </c>
-      <c r="J14">
-        <v>89.034904477952068</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>22.686011622165676</v>
+        <v>23.55197690759239</v>
       </c>
       <c r="C15">
-        <v>31.858407079646021</v>
+        <v>31.505184397432494</v>
       </c>
       <c r="D15">
-        <v>44.232595237190928</v>
+        <v>47.206502335827416</v>
       </c>
       <c r="E15">
-        <v>105.87565042348741</v>
+        <v>84.24930684796233</v>
       </c>
       <c r="F15">
-        <v>108.22287211819668</v>
+        <v>101.10144707356908</v>
       </c>
       <c r="G15">
-        <v>115.08222872118196</v>
+        <v>102.58270348285161</v>
       </c>
       <c r="H15">
-        <v>150.60959398382013</v>
+        <v>117.65733601731931</v>
       </c>
       <c r="I15">
-        <v>104.15511413270539</v>
+        <v>102.48015496220897</v>
       </c>
       <c r="J15">
-        <v>100.25827034828517</v>
+        <v>89.034904477952068</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>22.686011622165676</v>
+      </c>
+      <c r="C16">
+        <v>31.858407079646021</v>
+      </c>
+      <c r="D16">
+        <v>44.232595237190928</v>
+      </c>
+      <c r="E16">
+        <v>105.87565042348741</v>
+      </c>
+      <c r="F16">
+        <v>108.22287211819668</v>
+      </c>
+      <c r="G16">
+        <v>115.08222872118196</v>
+      </c>
+      <c r="H16">
+        <v>150.60959398382013</v>
+      </c>
+      <c r="I16">
+        <v>104.15511413270539</v>
+      </c>
+      <c r="J16">
+        <v>100.25827034828517</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>23.665919708306433</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>33.57894337042805</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>47.138136655398995</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>82.984541760036464</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>110.68403661361998</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>107.78988947548331</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>112.56409282540164</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>96.988111967792165</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>113.16798966918607</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <f>175/3</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="C18" s="2">
-        <f>B18/3</f>
+      <c r="C19" s="2">
+        <f>B19/3</f>
         <v>19.444444444444446</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" ref="D18:G18" si="3">C18/3</f>
+      <c r="D19" s="2">
+        <f t="shared" ref="D19:G19" si="3">C19/3</f>
         <v>6.4814814814814818</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <f t="shared" si="3"/>
         <v>2.1604938271604941</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <f t="shared" si="3"/>
         <v>0.72016460905349799</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="2">
         <f t="shared" si="3"/>
         <v>0.24005486968449932</v>
       </c>
-      <c r="H18" s="2">
-        <f>G18/3</f>
+      <c r="H19" s="2">
+        <f>G19/3</f>
         <v>8.0018289894833103E-2</v>
       </c>
-      <c r="I18" s="2">
-        <f>H18/3</f>
+      <c r="I19" s="2">
+        <f>H19/3</f>
         <v>2.66727632982777E-2</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>24.813619672860803</v>
-      </c>
-      <c r="C19">
-        <v>33.270279292311116</v>
-      </c>
-      <c r="D19">
-        <v>53.043284744631137</v>
-      </c>
-      <c r="E19">
-        <v>102.62601535551352</v>
-      </c>
-      <c r="F19">
-        <v>128.98631356403695</v>
-      </c>
-      <c r="G19">
-        <v>103.18237454100367</v>
-      </c>
-      <c r="H19">
-        <v>127.91810392789584</v>
-      </c>
-      <c r="I19">
-        <v>113.94236118838323</v>
-      </c>
-      <c r="J19">
-        <v>131.70134638922889</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>27.228218537888061</v>
+        <v>24.813619672860803</v>
       </c>
       <c r="C20">
-        <v>34.850339379103154</v>
+        <v>33.270279292311116</v>
       </c>
       <c r="D20">
-        <v>45.71047067987093</v>
+        <v>53.043284744631137</v>
       </c>
       <c r="E20">
-        <v>94.135974184933801</v>
+        <v>102.62601535551352</v>
       </c>
       <c r="F20">
-        <v>129.57605430065652</v>
+        <v>128.98631356403695</v>
       </c>
       <c r="G20">
-        <v>106.65405585846224</v>
+        <v>103.18237454100367</v>
       </c>
       <c r="H20">
-        <v>159.87537554245023</v>
+        <v>127.91810392789584</v>
       </c>
       <c r="I20">
-        <v>115.6782018471125</v>
+        <v>113.94236118838323</v>
       </c>
       <c r="J20">
-        <v>79.759652831868252</v>
+        <v>131.70134638922889</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>27.228218537888061</v>
+      </c>
+      <c r="C21">
+        <v>34.850339379103154</v>
+      </c>
+      <c r="D21">
+        <v>45.71047067987093</v>
+      </c>
+      <c r="E21">
+        <v>94.135974184933801</v>
+      </c>
+      <c r="F21">
+        <v>129.57605430065652</v>
+      </c>
+      <c r="G21">
+        <v>106.65405585846224</v>
+      </c>
+      <c r="H21">
+        <v>159.87537554245023</v>
+      </c>
+      <c r="I21">
+        <v>115.6782018471125</v>
+      </c>
+      <c r="J21">
+        <v>79.759652831868252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>28.085011683542898</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>34.071436519416942</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>48.492266607321696</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>86.19116501613442</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>117.93702014020253</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>105.27428507844665</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>116.23456103260266</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>121.35306553911207</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>99.543785467898076</v>
       </c>
     </row>

</xml_diff>